<commit_message>
Fix pausing, switch to "react" from "next" mode
</commit_message>
<xml_diff>
--- a/tolstoy_bot/botanik.xlsx
+++ b/tolstoy_bot/botanik.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
   <si>
     <t xml:space="preserve">Отправляйтесь на следующую локацию! Будем ждать вас по адресу Моховая 9 стр. 1 около здания МГУ. Когда прибудете на место, дайте нам знать (скиньте location).
 </t>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>На вопрос о наличии у вас велосипеда, пожалуйста, ответьте "да" или "нет"</t>
+  </si>
+  <si>
+    <t>[pause]</t>
   </si>
 </sst>
 </file>
@@ -771,7 +774,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -826,7 +829,7 @@
     </row>
     <row r="5" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>38</v>

</xml_diff>